<commit_message>
Update files to run through all steps in development env, issue #4
</commit_message>
<xml_diff>
--- a/workflow/CO-SWSI-Control.xlsx
+++ b/workflow/CO-SWSI-Control.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Water Supply Collaboration\SWSI WATF and Drought\SWSI monthly TSTool runs\2021-09\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Water Supply Collaboration\SWSI WATF and Drought\SWSI monthly TSTool runs\2022-06\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12525" yWindow="30" windowWidth="16005" windowHeight="12360" tabRatio="817" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="12525" yWindow="30" windowWidth="16005" windowHeight="12360" tabRatio="817" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Hist" sheetId="12" r:id="rId1"/>
@@ -1439,7 +1439,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5949" uniqueCount="1332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5994" uniqueCount="1345">
   <si>
     <t>HUC</t>
   </si>
@@ -5359,9 +5359,6 @@
     <t>MO - CACHE LA POUDRE R AT CANYON MOUTH, gage flow with calcs for major diversions by AAT</t>
   </si>
   <si>
-    <t>MO - SANGRE DE CRISTO, Data not loading, AAT</t>
-  </si>
-  <si>
     <t>2020-09</t>
   </si>
   <si>
@@ -5371,9 +5368,6 @@
     <t>2020-10</t>
   </si>
   <si>
-    <t>MO - RIVERSIDE RESERVOIR Data Not Loading AAT</t>
-  </si>
-  <si>
     <t>2020-11</t>
   </si>
   <si>
@@ -5383,9 +5377,6 @@
     <t>2021-01</t>
   </si>
   <si>
-    <t>MO - YAMCOLO RESERVOIR, DATA NOT LOADING by AAT</t>
-  </si>
-  <si>
     <t>2021-02</t>
   </si>
   <si>
@@ -5459,6 +5450,54 @@
   </si>
   <si>
     <t>MO - BOULDER CREEK NEAR ORODELL, gage flow with calcs for major diversions by TLK</t>
+  </si>
+  <si>
+    <t>2022-01</t>
+  </si>
+  <si>
+    <t>MO - SILVER JACK RESERVOIR, gage frozen, using last value</t>
+  </si>
+  <si>
+    <t>2022-02</t>
+  </si>
+  <si>
+    <t>2022-03</t>
+  </si>
+  <si>
+    <t>2022-04</t>
+  </si>
+  <si>
+    <t>2022-05</t>
+  </si>
+  <si>
+    <t>MO - SANGRE DE CRIST, Data not loading, AAT</t>
+  </si>
+  <si>
+    <t>MO - UTE CREEK, Data not loading, AAT</t>
+  </si>
+  <si>
+    <t>MO - RIO GRANDE NEAR DEL NORTE, data not the same as previous month, AAT</t>
+  </si>
+  <si>
+    <t>MO - ALAMOSA CREEK ABOVE TERRACE RESERVOIR, data not the same as previous month, AAT</t>
+  </si>
+  <si>
+    <t>MO - TRINCHERA CK, data not the same as previous month, AAT</t>
+  </si>
+  <si>
+    <t>MO - SANGRE DE CRISTO, data not the same as previous month, AAT</t>
+  </si>
+  <si>
+    <t>MO - UTE CREEK, data not the same as previous month, AAT</t>
+  </si>
+  <si>
+    <t>MO - CULEBRA CREEK AT SAN LUIS, data not the same as previous month, AAT</t>
+  </si>
+  <si>
+    <t>MO - SAGUACHE CREEK NEAR SAGUACHE, CO, data not the same as previous month, AAT</t>
+  </si>
+  <si>
+    <t>MO - CONEJOS RIVER NEAR MOGOTE, data not the same as previous month, AAT</t>
   </si>
 </sst>
 </file>
@@ -5923,7 +5962,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="155">
+  <cellXfs count="154">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -6108,7 +6147,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="30" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="47">
     <cellStyle name="Bad" xfId="25" builtinId="27"/>
@@ -8856,7 +8894,7 @@
       </c>
       <c r="T3" s="56" t="str">
         <f>RecentPeriodEndDateText</f>
-        <v>2020-09</v>
+        <v>2021-09</v>
       </c>
       <c r="V3" s="57" t="s">
         <v>883</v>
@@ -8925,11 +8963,11 @@
       </c>
       <c r="S4" s="56" t="str">
         <f>CurrentWaterYearStartDateText</f>
-        <v>2020-10</v>
+        <v>2021-10</v>
       </c>
       <c r="T4" s="56" t="str">
         <f>PreviousMonthDateText</f>
-        <v>2021-08</v>
+        <v>2022-05</v>
       </c>
       <c r="W4" s="58" t="s">
         <v>882</v>
@@ -8989,11 +9027,11 @@
       </c>
       <c r="S5" s="56" t="str">
         <f>CurrentMonthDateText</f>
-        <v>2021-09</v>
+        <v>2022-06</v>
       </c>
       <c r="T5" s="56" t="str">
         <f>CurrentMonthDateText</f>
-        <v>2021-09</v>
+        <v>2022-06</v>
       </c>
       <c r="W5" s="58" t="s">
         <v>883</v>
@@ -11113,8 +11151,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -11173,11 +11211,11 @@
         <v>512</v>
       </c>
       <c r="E7" s="10">
-        <v>44440</v>
+        <v>44713</v>
       </c>
       <c r="F7" s="9" t="str">
         <f>TEXT(CurrentMonthDate,"yyyy-mm")</f>
-        <v>2021-09</v>
+        <v>2022-06</v>
       </c>
       <c r="G7" t="s">
         <v>534</v>
@@ -11192,11 +11230,11 @@
       </c>
       <c r="E8" s="11">
         <f>MONTH(CurrentMonthDate)</f>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F8" s="11" t="str">
         <f>TEXT(CurrentMonthDate,"mm")</f>
-        <v>09</v>
+        <v>06</v>
       </c>
       <c r="G8" t="s">
         <v>533</v>
@@ -11211,11 +11249,11 @@
       </c>
       <c r="E9" s="9">
         <f>IF(MONTH(CurrentMonthDate)=1,DATE((YEAR(CurrentMonthDate)-1),12,1),DATE(YEAR(CurrentMonthDate),(MONTH(CurrentMonthDate)-1),1))</f>
-        <v>44409</v>
+        <v>44682</v>
       </c>
       <c r="F9" s="9" t="str">
         <f>TEXT(PreviousMonthDate,"yyyy-mm")</f>
-        <v>2021-08</v>
+        <v>2022-05</v>
       </c>
       <c r="G9" t="s">
         <v>532</v>
@@ -11230,11 +11268,11 @@
       </c>
       <c r="E10" s="9">
         <f>DATE(YEAR(CurrentMonthDate)-1,MONTH(CurrentMonthDate),1)</f>
-        <v>44075</v>
+        <v>44348</v>
       </c>
       <c r="F10" s="9" t="str">
         <f>TEXT(PreviousYearMonthDate,"yyyy-mm")</f>
-        <v>2020-09</v>
+        <v>2021-06</v>
       </c>
       <c r="G10" t="s">
         <v>832</v>
@@ -11247,9 +11285,9 @@
       <c r="D11" s="6" t="s">
         <v>512</v>
       </c>
-      <c r="E11" s="37" t="e">
+      <c r="E11" s="37" t="str">
         <f>VLOOKUP(CurrentMonth,SWSIForecastPeriodByMonth,2,FALSE)</f>
-        <v>#N/A</v>
+        <v>JUN-JUL</v>
       </c>
       <c r="F11" s="13"/>
       <c r="G11" t="s">
@@ -11263,9 +11301,9 @@
       <c r="D12" s="6" t="s">
         <v>512</v>
       </c>
-      <c r="E12" s="37" t="e">
+      <c r="E12" s="37" t="str">
         <f>VLOOKUP(CurrentMonth,SWSIForecastPeriodByMonth,3,FALSE)</f>
-        <v>#N/A</v>
+        <v>JUN-SEP</v>
       </c>
       <c r="F12" s="13"/>
       <c r="G12" t="s">
@@ -11289,11 +11327,11 @@
       </c>
       <c r="E14" s="38">
         <f>IF(MONTH(CurrentMonthDate)&lt;=9,DATE(YEAR(CurrentMonthDate)-1,10,1),DATE(YEAR(CurrentMonthDate),10,1))</f>
-        <v>44105</v>
+        <v>44470</v>
       </c>
       <c r="F14" s="9" t="str">
         <f>TEXT(CurrentWaterYearStartDate,"yyyy-mm")</f>
-        <v>2020-10</v>
+        <v>2021-10</v>
       </c>
       <c r="G14" t="s">
         <v>1045</v>
@@ -11309,11 +11347,11 @@
       </c>
       <c r="E15" s="32">
         <f>YEAR(CurrentWaterYearStartDate)+MONTH(CurrentWaterYearStartDate)/12</f>
-        <v>2020.8333333333333</v>
+        <v>2021.8333333333333</v>
       </c>
       <c r="F15" s="9" t="str">
         <f>TEXT(CurrentWaterYearStartDateDecimal,"#.##")</f>
-        <v>2020.83</v>
+        <v>2021.83</v>
       </c>
       <c r="G15" t="s">
         <v>1046</v>
@@ -11329,11 +11367,11 @@
       </c>
       <c r="E16" s="32">
         <f>CurrentWaterYearStartDateDecimal+0.1</f>
-        <v>2020.9333333333332</v>
+        <v>2021.9333333333332</v>
       </c>
       <c r="F16" s="9" t="str">
         <f>TEXT(CurrentPeriodAnnotationDecimal,"#.##")</f>
-        <v>2020.93</v>
+        <v>2021.93</v>
       </c>
       <c r="G16" t="s">
         <v>1047</v>
@@ -11348,11 +11386,11 @@
       </c>
       <c r="E17" s="9">
         <f>DATE((YEAR(CurrentWaterYearStartDate)+1),9,30)</f>
-        <v>44469</v>
+        <v>44834</v>
       </c>
       <c r="F17" s="9" t="str">
         <f>TEXT(CurrentWaterYearEndDate,"yyyy-mm")</f>
-        <v>2021-09</v>
+        <v>2022-09</v>
       </c>
       <c r="G17" t="s">
         <v>549</v>
@@ -11460,11 +11498,11 @@
       </c>
       <c r="E23" s="9">
         <f>CurrentWaterYearStartDate-1</f>
-        <v>44104</v>
+        <v>44469</v>
       </c>
       <c r="F23" s="9" t="str">
         <f>TEXT(RecentPeriodEndDate,"yyyy-mm")</f>
-        <v>2020-09</v>
+        <v>2021-09</v>
       </c>
       <c r="G23" t="s">
         <v>732</v>
@@ -11558,11 +11596,11 @@
       </c>
       <c r="E29" s="9">
         <f>CurrentWaterYearEndDate</f>
-        <v>44469</v>
+        <v>44834</v>
       </c>
       <c r="F29" s="9" t="str">
         <f>TEXT(InputPeriodEndDate,"yyyy-mm")</f>
-        <v>2021-09</v>
+        <v>2022-09</v>
       </c>
       <c r="G29" t="s">
         <v>726</v>
@@ -11577,11 +11615,11 @@
       </c>
       <c r="E30" s="9">
         <f>CurrentWaterYearEndDate</f>
-        <v>44469</v>
+        <v>44834</v>
       </c>
       <c r="F30" s="9" t="str">
         <f>TEXT(CurrentWaterYearEndDate,"yyyy-mm-dd")</f>
-        <v>2021-09-30</v>
+        <v>2022-09-30</v>
       </c>
       <c r="G30" t="s">
         <v>725</v>
@@ -11614,11 +11652,11 @@
       </c>
       <c r="E32" s="9">
         <f>CurrentWaterYearEndDate</f>
-        <v>44469</v>
+        <v>44834</v>
       </c>
       <c r="F32" s="9" t="str">
         <f>TEXT(RecentPeriodGraphEndDate,"yyyy-mm")</f>
-        <v>2021-09</v>
+        <v>2022-09</v>
       </c>
       <c r="G32" t="s">
         <v>547</v>
@@ -11677,7 +11715,7 @@
         <v>512</v>
       </c>
       <c r="E37" s="123" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="F37" s="8"/>
       <c r="G37" t="s">
@@ -26795,7 +26833,7 @@
       </c>
       <c r="H2" s="44" t="str">
         <f t="shared" ref="H2:H10" si="1">RecentPeriodEndDateText</f>
-        <v>2020-09</v>
+        <v>2021-09</v>
       </c>
       <c r="I2" s="44" t="s">
         <v>885</v>
@@ -26826,7 +26864,7 @@
       </c>
       <c r="H3" s="44" t="str">
         <f t="shared" si="1"/>
-        <v>2020-09</v>
+        <v>2021-09</v>
       </c>
       <c r="I3" s="44" t="s">
         <v>886</v>
@@ -26858,7 +26896,7 @@
       </c>
       <c r="H4" s="44" t="str">
         <f t="shared" si="1"/>
-        <v>2020-09</v>
+        <v>2021-09</v>
       </c>
       <c r="I4" s="44" t="s">
         <v>692</v>
@@ -26903,7 +26941,7 @@
       </c>
       <c r="H5" s="44" t="str">
         <f t="shared" si="1"/>
-        <v>2020-09</v>
+        <v>2021-09</v>
       </c>
       <c r="I5" s="46" t="s">
         <v>999</v>
@@ -26946,7 +26984,7 @@
       </c>
       <c r="H6" s="44" t="str">
         <f t="shared" si="1"/>
-        <v>2020-09</v>
+        <v>2021-09</v>
       </c>
       <c r="I6" s="44" t="s">
         <v>691</v>
@@ -26977,7 +27015,7 @@
       </c>
       <c r="H7" s="44" t="str">
         <f t="shared" si="1"/>
-        <v>2020-09</v>
+        <v>2021-09</v>
       </c>
       <c r="I7" s="44" t="s">
         <v>692</v>
@@ -27008,7 +27046,7 @@
       </c>
       <c r="H8" s="44" t="str">
         <f t="shared" si="1"/>
-        <v>2020-09</v>
+        <v>2021-09</v>
       </c>
       <c r="I8" s="44" t="s">
         <v>692</v>
@@ -27039,7 +27077,7 @@
       </c>
       <c r="H9" s="44" t="str">
         <f t="shared" si="1"/>
-        <v>2020-09</v>
+        <v>2021-09</v>
       </c>
       <c r="I9" s="44" t="s">
         <v>692</v>
@@ -27071,7 +27109,7 @@
       </c>
       <c r="H10" s="44" t="str">
         <f t="shared" si="1"/>
-        <v>2020-09</v>
+        <v>2021-09</v>
       </c>
       <c r="I10" s="44" t="s">
         <v>704</v>
@@ -27131,7 +27169,7 @@
       </c>
       <c r="H12" s="80" t="str">
         <f>CurrentMonthDateText</f>
-        <v>2021-09</v>
+        <v>2022-06</v>
       </c>
       <c r="I12" s="44" t="s">
         <v>887</v>
@@ -27163,7 +27201,7 @@
       </c>
       <c r="H13" s="44" t="str">
         <f t="shared" ref="H13:H24" si="3">RecentPeriodEndDateText</f>
-        <v>2020-09</v>
+        <v>2021-09</v>
       </c>
       <c r="I13" s="44" t="s">
         <v>704</v>
@@ -27195,7 +27233,7 @@
       </c>
       <c r="H14" s="44" t="str">
         <f t="shared" si="3"/>
-        <v>2020-09</v>
+        <v>2021-09</v>
       </c>
       <c r="I14" s="44" t="s">
         <v>710</v>
@@ -27226,7 +27264,7 @@
       </c>
       <c r="H15" s="44" t="str">
         <f t="shared" si="3"/>
-        <v>2020-09</v>
+        <v>2021-09</v>
       </c>
       <c r="I15" s="44" t="s">
         <v>692</v>
@@ -27258,7 +27296,7 @@
       </c>
       <c r="H16" s="44" t="str">
         <f t="shared" si="3"/>
-        <v>2020-09</v>
+        <v>2021-09</v>
       </c>
       <c r="I16" s="44" t="s">
         <v>692</v>
@@ -27290,7 +27328,7 @@
       </c>
       <c r="H17" s="44" t="str">
         <f t="shared" si="3"/>
-        <v>2020-09</v>
+        <v>2021-09</v>
       </c>
       <c r="I17" s="44" t="s">
         <v>692</v>
@@ -27321,7 +27359,7 @@
       </c>
       <c r="H18" s="44" t="str">
         <f t="shared" si="3"/>
-        <v>2020-09</v>
+        <v>2021-09</v>
       </c>
       <c r="I18" s="39" t="s">
         <v>888</v>
@@ -27353,7 +27391,7 @@
       </c>
       <c r="H19" s="44" t="str">
         <f t="shared" si="3"/>
-        <v>2020-09</v>
+        <v>2021-09</v>
       </c>
       <c r="I19" s="44" t="s">
         <v>692</v>
@@ -27385,7 +27423,7 @@
       </c>
       <c r="H20" s="44" t="str">
         <f t="shared" si="3"/>
-        <v>2020-09</v>
+        <v>2021-09</v>
       </c>
       <c r="I20" s="44" t="s">
         <v>889</v>
@@ -27416,7 +27454,7 @@
       </c>
       <c r="H21" s="44" t="str">
         <f t="shared" si="3"/>
-        <v>2020-09</v>
+        <v>2021-09</v>
       </c>
       <c r="I21" s="44" t="s">
         <v>1061</v>
@@ -27447,7 +27485,7 @@
       </c>
       <c r="H22" s="44" t="str">
         <f t="shared" si="3"/>
-        <v>2020-09</v>
+        <v>2021-09</v>
       </c>
       <c r="I22" s="44" t="s">
         <v>692</v>
@@ -27479,7 +27517,7 @@
       </c>
       <c r="H23" s="44" t="str">
         <f t="shared" si="3"/>
-        <v>2020-09</v>
+        <v>2021-09</v>
       </c>
       <c r="I23" s="44" t="s">
         <v>890</v>
@@ -27511,7 +27549,7 @@
       </c>
       <c r="H24" s="44" t="str">
         <f t="shared" si="3"/>
-        <v>2020-09</v>
+        <v>2021-09</v>
       </c>
       <c r="I24" s="44" t="s">
         <v>891</v>
@@ -27573,7 +27611,7 @@
       </c>
       <c r="H26" s="44" t="str">
         <f t="shared" ref="H26:H35" si="4">RecentPeriodEndDateText</f>
-        <v>2020-09</v>
+        <v>2021-09</v>
       </c>
       <c r="I26" s="44" t="s">
         <v>700</v>
@@ -27605,7 +27643,7 @@
       </c>
       <c r="H27" s="44" t="str">
         <f t="shared" si="4"/>
-        <v>2020-09</v>
+        <v>2021-09</v>
       </c>
       <c r="I27" s="44" t="s">
         <v>705</v>
@@ -27637,7 +27675,7 @@
       </c>
       <c r="H28" s="44" t="str">
         <f t="shared" si="4"/>
-        <v>2020-09</v>
+        <v>2021-09</v>
       </c>
       <c r="I28" s="44" t="s">
         <v>892</v>
@@ -27669,7 +27707,7 @@
       </c>
       <c r="H29" s="44" t="str">
         <f t="shared" si="4"/>
-        <v>2020-09</v>
+        <v>2021-09</v>
       </c>
       <c r="I29" s="44" t="s">
         <v>893</v>
@@ -27701,7 +27739,7 @@
       </c>
       <c r="H30" s="80" t="str">
         <f>CurrentMonthDateText</f>
-        <v>2021-09</v>
+        <v>2022-06</v>
       </c>
       <c r="I30" s="44" t="s">
         <v>689</v>
@@ -27733,7 +27771,7 @@
       </c>
       <c r="H31" s="44" t="str">
         <f t="shared" si="4"/>
-        <v>2020-09</v>
+        <v>2021-09</v>
       </c>
       <c r="I31" s="44" t="s">
         <v>894</v>
@@ -27764,7 +27802,7 @@
       </c>
       <c r="H32" s="44" t="str">
         <f t="shared" si="4"/>
-        <v>2020-09</v>
+        <v>2021-09</v>
       </c>
       <c r="I32" s="44" t="s">
         <v>692</v>
@@ -27796,7 +27834,7 @@
       </c>
       <c r="H33" s="44" t="str">
         <f t="shared" si="4"/>
-        <v>2020-09</v>
+        <v>2021-09</v>
       </c>
       <c r="I33" s="44" t="s">
         <v>895</v>
@@ -27828,7 +27866,7 @@
       </c>
       <c r="H34" s="44" t="str">
         <f t="shared" si="4"/>
-        <v>2020-09</v>
+        <v>2021-09</v>
       </c>
       <c r="I34" s="44" t="s">
         <v>896</v>
@@ -27860,7 +27898,7 @@
       </c>
       <c r="H35" s="44" t="str">
         <f t="shared" si="4"/>
-        <v>2020-09</v>
+        <v>2021-09</v>
       </c>
       <c r="I35" s="44" t="s">
         <v>897</v>
@@ -28649,10 +28687,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U2799"/>
+  <dimension ref="A1:U2791"/>
   <sheetViews>
-    <sheetView topLeftCell="A157" workbookViewId="0">
-      <selection activeCell="A287" sqref="A287"/>
+    <sheetView tabSelected="1" topLeftCell="A279" workbookViewId="0">
+      <selection activeCell="F306" sqref="F306"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -31181,7 +31219,7 @@
         <v>628</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="D147" s="1" t="s">
         <v>687</v>
@@ -31198,7 +31236,7 @@
         <v>628</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
       <c r="D148" s="1" t="s">
         <v>687</v>
@@ -31215,7 +31253,7 @@
         <v>628</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>1303</v>
+        <v>1301</v>
       </c>
       <c r="D149" s="1" t="s">
         <v>687</v>
@@ -31232,7 +31270,7 @@
         <v>628</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>1304</v>
+        <v>1302</v>
       </c>
       <c r="D150" s="1" t="s">
         <v>687</v>
@@ -31249,7 +31287,7 @@
         <v>628</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>1305</v>
+        <v>1303</v>
       </c>
       <c r="D151" s="1" t="s">
         <v>687</v>
@@ -31266,7 +31304,7 @@
         <v>628</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>1307</v>
+        <v>1304</v>
       </c>
       <c r="D152" s="1" t="s">
         <v>687</v>
@@ -31283,7 +31321,7 @@
         <v>628</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>1308</v>
+        <v>1305</v>
       </c>
       <c r="D153" s="1" t="s">
         <v>687</v>
@@ -31300,7 +31338,7 @@
         <v>628</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>1317</v>
+        <v>1314</v>
       </c>
       <c r="D154" s="1" t="s">
         <v>687</v>
@@ -31317,7 +31355,7 @@
         <v>628</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>1318</v>
+        <v>1315</v>
       </c>
       <c r="D155" s="1" t="s">
         <v>687</v>
@@ -31334,7 +31372,7 @@
         <v>628</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>1319</v>
+        <v>1316</v>
       </c>
       <c r="D156" s="1" t="s">
         <v>687</v>
@@ -33079,7 +33117,7 @@
         <v>628</v>
       </c>
       <c r="C258" s="1" t="s">
-        <v>1321</v>
+        <v>1318</v>
       </c>
       <c r="D258" s="1" t="s">
         <v>687</v>
@@ -33096,7 +33134,7 @@
         <v>633</v>
       </c>
       <c r="C259" s="1" t="s">
-        <v>1319</v>
+        <v>1316</v>
       </c>
       <c r="D259" s="138" t="s">
         <v>206</v>
@@ -33105,7 +33143,7 @@
         <v>26503</v>
       </c>
       <c r="F259" s="138" t="s">
-        <v>1309</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="260" spans="1:6">
@@ -33125,7 +33163,7 @@
         <v>0</v>
       </c>
       <c r="F260" s="138" t="s">
-        <v>1310</v>
+        <v>1307</v>
       </c>
     </row>
     <row r="261" spans="1:6">
@@ -33145,7 +33183,7 @@
         <v>180</v>
       </c>
       <c r="F261" s="138" t="s">
-        <v>1311</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="262" spans="1:6">
@@ -33154,7 +33192,7 @@
         <v>633</v>
       </c>
       <c r="C262" s="1" t="s">
-        <v>1319</v>
+        <v>1316</v>
       </c>
       <c r="D262" s="138" t="s">
         <v>228</v>
@@ -33163,7 +33201,7 @@
         <v>38600</v>
       </c>
       <c r="F262" s="138" t="s">
-        <v>1320</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="263" spans="1:6">
@@ -33183,7 +33221,7 @@
         <v>88</v>
       </c>
       <c r="F263" s="138" t="s">
-        <v>1312</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="264" spans="1:6">
@@ -33203,7 +33241,7 @@
         <v>54</v>
       </c>
       <c r="F264" s="138" t="s">
-        <v>1313</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="265" spans="1:6">
@@ -33223,7 +33261,7 @@
         <v>54</v>
       </c>
       <c r="F265" s="138" t="s">
-        <v>1314</v>
+        <v>1311</v>
       </c>
     </row>
     <row r="266" spans="1:6">
@@ -33243,7 +33281,7 @@
         <v>90</v>
       </c>
       <c r="F266" s="138" t="s">
-        <v>1315</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="267" spans="1:6">
@@ -33263,7 +33301,7 @@
         <v>225</v>
       </c>
       <c r="F267" s="138" t="s">
-        <v>1316</v>
+        <v>1313</v>
       </c>
     </row>
     <row r="268" spans="1:6">
@@ -33271,7 +33309,7 @@
         <v>633</v>
       </c>
       <c r="C268" s="1" t="s">
-        <v>1319</v>
+        <v>1316</v>
       </c>
       <c r="D268" s="138" t="s">
         <v>359</v>
@@ -33288,7 +33326,7 @@
         <v>633</v>
       </c>
       <c r="C269" s="1" t="s">
-        <v>1319</v>
+        <v>1316</v>
       </c>
       <c r="D269" s="138" t="s">
         <v>341</v>
@@ -33305,7 +33343,7 @@
         <v>633</v>
       </c>
       <c r="C270" s="1" t="s">
-        <v>1319</v>
+        <v>1316</v>
       </c>
       <c r="D270" s="138" t="s">
         <v>242</v>
@@ -33323,7 +33361,7 @@
         <v>633</v>
       </c>
       <c r="C271" s="1" t="s">
-        <v>1319</v>
+        <v>1316</v>
       </c>
       <c r="D271" s="138" t="s">
         <v>243</v>
@@ -33337,11 +33375,21 @@
     </row>
     <row r="272" spans="1:6">
       <c r="A272" s="138"/>
-      <c r="B272" s="138"/>
-      <c r="C272" s="1"/>
-      <c r="D272" s="138"/>
-      <c r="E272" s="152"/>
-      <c r="F272" s="138"/>
+      <c r="B272" s="138" t="s">
+        <v>628</v>
+      </c>
+      <c r="C272" s="1" t="s">
+        <v>1331</v>
+      </c>
+      <c r="D272" s="1" t="s">
+        <v>687</v>
+      </c>
+      <c r="E272" s="152">
+        <v>666</v>
+      </c>
+      <c r="F272" s="138" t="s">
+        <v>1167</v>
+      </c>
     </row>
     <row r="273" spans="1:6">
       <c r="A273" s="138"/>
@@ -33349,7 +33397,7 @@
         <v>628</v>
       </c>
       <c r="C273" s="1" t="s">
-        <v>1327</v>
+        <v>1324</v>
       </c>
       <c r="D273" s="1" t="s">
         <v>687</v>
@@ -33367,7 +33415,7 @@
         <v>628</v>
       </c>
       <c r="C274" s="1" t="s">
-        <v>1325</v>
+        <v>1322</v>
       </c>
       <c r="D274" s="1" t="s">
         <v>687</v>
@@ -33376,7 +33424,7 @@
         <v>0.9</v>
       </c>
       <c r="F274" s="138" t="s">
-        <v>1326</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="275" spans="1:6">
@@ -33385,7 +33433,7 @@
         <v>628</v>
       </c>
       <c r="C275" s="1" t="s">
-        <v>1324</v>
+        <v>1321</v>
       </c>
       <c r="D275" s="1" t="s">
         <v>687</v>
@@ -33403,7 +33451,7 @@
         <v>628</v>
       </c>
       <c r="C276" s="1" t="s">
-        <v>1323</v>
+        <v>1320</v>
       </c>
       <c r="D276" s="1" t="s">
         <v>687</v>
@@ -33421,7 +33469,7 @@
         <v>628</v>
       </c>
       <c r="C277" s="1" t="s">
-        <v>1322</v>
+        <v>1319</v>
       </c>
       <c r="D277" s="1" t="s">
         <v>687</v>
@@ -33434,23 +33482,20 @@
       </c>
     </row>
     <row r="278" spans="1:6">
-      <c r="A278" t="s">
-        <v>550</v>
-      </c>
       <c r="B278" s="138" t="s">
-        <v>633</v>
+        <v>628</v>
       </c>
       <c r="C278" s="1" t="s">
-        <v>1293</v>
-      </c>
-      <c r="D278" s="138" t="s">
-        <v>359</v>
+        <v>1318</v>
+      </c>
+      <c r="D278" s="1" t="s">
+        <v>687</v>
       </c>
       <c r="E278" s="152">
-        <v>7223</v>
+        <v>549</v>
       </c>
       <c r="F278" s="138" t="s">
-        <v>1297</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="279" spans="1:6">
@@ -33471,83 +33516,73 @@
       </c>
     </row>
     <row r="280" spans="1:6">
-      <c r="A280" t="s">
-        <v>550</v>
-      </c>
       <c r="B280" s="138" t="s">
-        <v>633</v>
-      </c>
-      <c r="C280" s="139" t="s">
-        <v>1293</v>
-      </c>
-      <c r="D280" s="138" t="s">
-        <v>341</v>
+        <v>628</v>
+      </c>
+      <c r="C280" s="1" t="s">
+        <v>1329</v>
+      </c>
+      <c r="D280" s="1" t="s">
+        <v>687</v>
       </c>
       <c r="E280" s="152">
-        <v>3971</v>
+        <v>455</v>
       </c>
       <c r="F280" s="138" t="s">
-        <v>1294</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="281" spans="1:6">
-      <c r="A281" t="s">
-        <v>550</v>
-      </c>
       <c r="B281" s="138" t="s">
-        <v>633</v>
-      </c>
-      <c r="C281" s="139" t="s">
-        <v>1293</v>
-      </c>
-      <c r="D281" s="138" t="s">
-        <v>242</v>
+        <v>628</v>
+      </c>
+      <c r="C281" s="1" t="s">
+        <v>1332</v>
+      </c>
+      <c r="D281" s="1" t="s">
+        <v>687</v>
       </c>
       <c r="E281" s="152">
-        <v>6288</v>
+        <v>654</v>
       </c>
       <c r="F281" s="138" t="s">
-        <v>1295</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="282" spans="1:6">
-      <c r="A282" s="138" t="s">
-        <v>550</v>
-      </c>
+      <c r="A282" s="138"/>
       <c r="B282" s="138" t="s">
         <v>633</v>
       </c>
       <c r="C282" s="139" t="s">
         <v>1293</v>
       </c>
-      <c r="D282" s="138" t="s">
-        <v>243</v>
+      <c r="D282" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="E282" s="152">
-        <v>5584</v>
+        <v>0</v>
       </c>
       <c r="F282" s="138" t="s">
-        <v>1296</v>
+        <v>1299</v>
       </c>
     </row>
     <row r="283" spans="1:6">
-      <c r="A283" t="s">
-        <v>550</v>
-      </c>
+      <c r="A283" s="138"/>
       <c r="B283" s="138" t="s">
-        <v>633</v>
+        <v>628</v>
       </c>
       <c r="C283" s="139" t="s">
-        <v>1293</v>
-      </c>
-      <c r="D283" s="138" t="s">
-        <v>405</v>
+        <v>1333</v>
+      </c>
+      <c r="D283" s="1" t="s">
+        <v>687</v>
       </c>
       <c r="E283" s="152">
-        <v>50</v>
+        <v>549</v>
       </c>
       <c r="F283" s="138" t="s">
-        <v>1298</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="284" spans="1:6">
@@ -33555,57 +33590,53 @@
       <c r="B284" s="138" t="s">
         <v>633</v>
       </c>
-      <c r="C284" s="139" t="s">
-        <v>1293</v>
-      </c>
-      <c r="D284" s="1" t="s">
-        <v>3</v>
+      <c r="C284" s="1" t="s">
+        <v>1322</v>
+      </c>
+      <c r="D284" s="138" t="s">
+        <v>359</v>
       </c>
       <c r="E284" s="152">
-        <v>0</v>
+        <v>19116</v>
       </c>
       <c r="F284" s="138" t="s">
-        <v>1300</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="285" spans="1:6">
-      <c r="A285" s="138" t="s">
-        <v>550</v>
-      </c>
+      <c r="A285" s="138"/>
       <c r="B285" s="138" t="s">
-        <v>628</v>
-      </c>
-      <c r="C285" s="139" t="s">
-        <v>1301</v>
+        <v>633</v>
+      </c>
+      <c r="C285" s="1" t="s">
+        <v>1322</v>
       </c>
       <c r="D285" s="138" t="s">
-        <v>684</v>
+        <v>341</v>
       </c>
       <c r="E285" s="152">
-        <v>10754</v>
+        <v>11790</v>
       </c>
       <c r="F285" s="138" t="s">
-        <v>1302</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="286" spans="1:6">
-      <c r="A286" s="138" t="s">
-        <v>550</v>
-      </c>
+      <c r="A286" s="138"/>
       <c r="B286" s="138" t="s">
-        <v>628</v>
-      </c>
-      <c r="C286" s="139" t="s">
-        <v>1303</v>
+        <v>633</v>
+      </c>
+      <c r="C286" s="1" t="s">
+        <v>1322</v>
       </c>
       <c r="D286" s="138" t="s">
-        <v>684</v>
+        <v>242</v>
       </c>
       <c r="E286" s="152">
-        <v>24390</v>
+        <v>7552</v>
       </c>
       <c r="F286" s="138" t="s">
-        <v>1302</v>
+        <v>1327</v>
       </c>
     </row>
     <row r="287" spans="1:6">
@@ -33614,13 +33645,13 @@
         <v>633</v>
       </c>
       <c r="C287" s="1" t="s">
-        <v>1325</v>
+        <v>1322</v>
       </c>
       <c r="D287" s="138" t="s">
-        <v>359</v>
+        <v>243</v>
       </c>
       <c r="E287" s="152">
-        <v>19116</v>
+        <v>4620</v>
       </c>
       <c r="F287" s="138" t="s">
         <v>1328</v>
@@ -33629,34 +33660,34 @@
     <row r="288" spans="1:6">
       <c r="A288" s="138"/>
       <c r="B288" s="138" t="s">
-        <v>633</v>
-      </c>
-      <c r="C288" s="1" t="s">
-        <v>1325</v>
+        <v>628</v>
+      </c>
+      <c r="C288" s="139" t="s">
+        <v>1331</v>
       </c>
       <c r="D288" s="138" t="s">
-        <v>341</v>
+        <v>609</v>
       </c>
       <c r="E288" s="152">
-        <v>11790</v>
+        <v>1097</v>
       </c>
       <c r="F288" s="138" t="s">
-        <v>1329</v>
+        <v>1330</v>
       </c>
     </row>
     <row r="289" spans="1:6">
       <c r="A289" s="138"/>
       <c r="B289" s="138" t="s">
-        <v>633</v>
-      </c>
-      <c r="C289" s="1" t="s">
-        <v>1325</v>
+        <v>628</v>
+      </c>
+      <c r="C289" s="139" t="s">
+        <v>1329</v>
       </c>
       <c r="D289" s="138" t="s">
-        <v>242</v>
+        <v>609</v>
       </c>
       <c r="E289" s="152">
-        <v>7552</v>
+        <v>1097</v>
       </c>
       <c r="F289" s="138" t="s">
         <v>1330</v>
@@ -33665,111 +33696,231 @@
     <row r="290" spans="1:6">
       <c r="A290" s="138"/>
       <c r="B290" s="138" t="s">
-        <v>633</v>
-      </c>
-      <c r="C290" s="1" t="s">
-        <v>1325</v>
+        <v>628</v>
+      </c>
+      <c r="C290" s="139" t="s">
+        <v>1332</v>
       </c>
       <c r="D290" s="138" t="s">
-        <v>243</v>
+        <v>609</v>
       </c>
       <c r="E290" s="152">
-        <v>4620</v>
+        <v>1097</v>
       </c>
       <c r="F290" s="138" t="s">
-        <v>1331</v>
+        <v>1330</v>
       </c>
     </row>
     <row r="291" spans="1:6">
-      <c r="A291" s="138"/>
-      <c r="B291" s="138"/>
-      <c r="C291" s="139"/>
-      <c r="D291" s="138"/>
-      <c r="E291" s="152"/>
-      <c r="F291" s="138"/>
+      <c r="B291" s="138" t="s">
+        <v>628</v>
+      </c>
+      <c r="C291" s="139" t="s">
+        <v>1334</v>
+      </c>
+      <c r="D291" s="1" t="s">
+        <v>687</v>
+      </c>
+      <c r="E291" s="152">
+        <v>503</v>
+      </c>
+      <c r="F291" s="138" t="s">
+        <v>1167</v>
+      </c>
     </row>
     <row r="292" spans="1:6">
-      <c r="A292" s="138"/>
-      <c r="B292" s="138"/>
-      <c r="C292" s="139"/>
-      <c r="D292" s="138"/>
-      <c r="E292" s="152"/>
-      <c r="F292" s="138"/>
+      <c r="B292" s="138" t="s">
+        <v>634</v>
+      </c>
+      <c r="C292" s="139" t="s">
+        <v>1334</v>
+      </c>
+      <c r="D292" s="138" t="s">
+        <v>405</v>
+      </c>
+      <c r="E292" s="152">
+        <v>1620</v>
+      </c>
+      <c r="F292" s="138" t="s">
+        <v>1335</v>
+      </c>
     </row>
     <row r="293" spans="1:6">
-      <c r="A293" s="138"/>
-      <c r="B293" s="138"/>
-      <c r="C293" s="139"/>
-      <c r="D293" s="138"/>
-      <c r="E293" s="152"/>
-      <c r="F293" s="138"/>
+      <c r="B293" s="138" t="s">
+        <v>634</v>
+      </c>
+      <c r="C293" s="139" t="s">
+        <v>1334</v>
+      </c>
+      <c r="D293" s="138" t="s">
+        <v>399</v>
+      </c>
+      <c r="E293" s="152">
+        <v>3600</v>
+      </c>
+      <c r="F293" s="138" t="s">
+        <v>1336</v>
+      </c>
     </row>
     <row r="294" spans="1:6">
-      <c r="A294" s="138"/>
-      <c r="B294" s="138"/>
-      <c r="C294" s="154"/>
-      <c r="D294" s="138"/>
-      <c r="E294" s="152"/>
-      <c r="F294" s="138"/>
+      <c r="A294" t="s">
+        <v>550</v>
+      </c>
+      <c r="B294" s="138" t="s">
+        <v>634</v>
+      </c>
+      <c r="C294" s="139" t="s">
+        <v>1334</v>
+      </c>
+      <c r="D294" s="138" t="s">
+        <v>389</v>
+      </c>
+      <c r="E294" s="138">
+        <v>235000</v>
+      </c>
+      <c r="F294" s="138" t="s">
+        <v>1337</v>
+      </c>
     </row>
     <row r="295" spans="1:6">
-      <c r="B295" s="138"/>
-      <c r="C295" s="139"/>
-      <c r="D295" s="138"/>
-      <c r="E295" s="152"/>
-      <c r="F295" s="138"/>
+      <c r="A295" s="138" t="s">
+        <v>550</v>
+      </c>
+      <c r="B295" s="138" t="s">
+        <v>634</v>
+      </c>
+      <c r="C295" s="139" t="s">
+        <v>1334</v>
+      </c>
+      <c r="D295" s="138" t="s">
+        <v>401</v>
+      </c>
+      <c r="E295" s="138">
+        <v>40000</v>
+      </c>
+      <c r="F295" s="138" t="s">
+        <v>1338</v>
+      </c>
     </row>
     <row r="296" spans="1:6">
+      <c r="A296" s="138" t="s">
+        <v>550</v>
+      </c>
       <c r="B296" s="138" t="s">
-        <v>628</v>
+        <v>634</v>
       </c>
       <c r="C296" s="139" t="s">
-        <v>1305</v>
+        <v>1334</v>
       </c>
       <c r="D296" s="138" t="s">
-        <v>478</v>
-      </c>
-      <c r="E296" s="152">
-        <v>4610</v>
+        <v>407</v>
+      </c>
+      <c r="E296" s="138">
+        <v>3200</v>
       </c>
       <c r="F296" s="138" t="s">
-        <v>1306</v>
+        <v>1339</v>
       </c>
     </row>
     <row r="297" spans="1:6">
-      <c r="B297" s="138"/>
-      <c r="C297" s="139"/>
-      <c r="D297" s="138"/>
-      <c r="E297" s="152"/>
-      <c r="F297" s="138"/>
+      <c r="A297" s="138" t="s">
+        <v>550</v>
+      </c>
+      <c r="B297" s="138" t="s">
+        <v>634</v>
+      </c>
+      <c r="C297" s="139" t="s">
+        <v>1334</v>
+      </c>
+      <c r="D297" s="138" t="s">
+        <v>405</v>
+      </c>
+      <c r="E297" s="138">
+        <v>1620</v>
+      </c>
+      <c r="F297" s="138" t="s">
+        <v>1340</v>
+      </c>
     </row>
     <row r="298" spans="1:6">
-      <c r="B298" s="138"/>
-      <c r="C298" s="138"/>
-      <c r="D298" s="1"/>
-      <c r="E298" s="138"/>
-      <c r="F298" s="138"/>
+      <c r="A298" s="138" t="s">
+        <v>550</v>
+      </c>
+      <c r="B298" s="138" t="s">
+        <v>634</v>
+      </c>
+      <c r="C298" s="139" t="s">
+        <v>1334</v>
+      </c>
+      <c r="D298" s="138" t="s">
+        <v>399</v>
+      </c>
+      <c r="E298" s="138">
+        <v>3600</v>
+      </c>
+      <c r="F298" s="138" t="s">
+        <v>1341</v>
+      </c>
     </row>
     <row r="299" spans="1:6">
-      <c r="B299" s="138"/>
-      <c r="C299" s="138"/>
-      <c r="D299" s="1"/>
-      <c r="E299" s="138"/>
-      <c r="F299" s="138"/>
+      <c r="A299" s="138" t="s">
+        <v>550</v>
+      </c>
+      <c r="B299" s="138" t="s">
+        <v>634</v>
+      </c>
+      <c r="C299" s="139" t="s">
+        <v>1334</v>
+      </c>
+      <c r="D299" s="138" t="s">
+        <v>403</v>
+      </c>
+      <c r="E299" s="138">
+        <v>5700</v>
+      </c>
+      <c r="F299" s="138" t="s">
+        <v>1342</v>
+      </c>
     </row>
     <row r="300" spans="1:6">
-      <c r="B300" s="138"/>
-      <c r="C300" s="138"/>
-      <c r="D300" s="1"/>
-      <c r="E300" s="138"/>
-      <c r="F300" s="138"/>
+      <c r="A300" s="138" t="s">
+        <v>550</v>
+      </c>
+      <c r="B300" s="138" t="s">
+        <v>634</v>
+      </c>
+      <c r="C300" s="139" t="s">
+        <v>1334</v>
+      </c>
+      <c r="D300" s="138" t="s">
+        <v>409</v>
+      </c>
+      <c r="E300" s="138">
+        <v>13500</v>
+      </c>
+      <c r="F300" s="138" t="s">
+        <v>1343</v>
+      </c>
     </row>
     <row r="301" spans="1:6">
-      <c r="B301" s="138"/>
-      <c r="C301" s="138"/>
-      <c r="D301" s="1"/>
-      <c r="E301" s="138"/>
-      <c r="F301" s="138"/>
+      <c r="A301" s="138" t="s">
+        <v>550</v>
+      </c>
+      <c r="B301" s="138" t="s">
+        <v>634</v>
+      </c>
+      <c r="C301" s="139" t="s">
+        <v>1334</v>
+      </c>
+      <c r="D301" s="138" t="s">
+        <v>411</v>
+      </c>
+      <c r="E301" s="138">
+        <v>120000</v>
+      </c>
+      <c r="F301" s="138" t="s">
+        <v>1344</v>
+      </c>
     </row>
     <row r="302" spans="1:6">
       <c r="B302" s="138"/>
@@ -35178,61 +35329,37 @@
       <c r="E502" s="138"/>
       <c r="F502" s="138"/>
     </row>
-    <row r="503" spans="2:6">
-      <c r="B503" s="138"/>
-      <c r="C503" s="138"/>
-      <c r="D503" s="1"/>
-      <c r="E503" s="138"/>
-      <c r="F503" s="138"/>
-    </row>
-    <row r="504" spans="2:6">
-      <c r="B504" s="138"/>
-      <c r="C504" s="138"/>
-      <c r="D504" s="1"/>
-      <c r="E504" s="138"/>
-      <c r="F504" s="138"/>
-    </row>
-    <row r="505" spans="2:6">
-      <c r="B505" s="138"/>
-      <c r="C505" s="138"/>
-      <c r="D505" s="1"/>
-      <c r="E505" s="138"/>
-      <c r="F505" s="138"/>
-    </row>
-    <row r="506" spans="2:6">
-      <c r="B506" s="138"/>
-      <c r="C506" s="138"/>
-      <c r="D506" s="1"/>
-      <c r="E506" s="138"/>
-      <c r="F506" s="138"/>
-    </row>
-    <row r="507" spans="2:6">
-      <c r="B507" s="138"/>
-      <c r="C507" s="138"/>
-      <c r="D507" s="1"/>
-      <c r="E507" s="138"/>
-      <c r="F507" s="138"/>
-    </row>
-    <row r="508" spans="2:6">
-      <c r="B508" s="138"/>
-      <c r="C508" s="138"/>
-      <c r="D508" s="1"/>
-      <c r="E508" s="138"/>
-      <c r="F508" s="138"/>
-    </row>
-    <row r="509" spans="2:6">
-      <c r="B509" s="138"/>
-      <c r="C509" s="138"/>
-      <c r="D509" s="1"/>
-      <c r="E509" s="138"/>
-      <c r="F509" s="138"/>
-    </row>
-    <row r="510" spans="2:6">
-      <c r="B510" s="138"/>
-      <c r="C510" s="138"/>
-      <c r="D510" s="1"/>
-      <c r="E510" s="138"/>
-      <c r="F510" s="138"/>
+    <row r="548" spans="3:4">
+      <c r="C548" s="1"/>
+      <c r="D548" s="1"/>
+    </row>
+    <row r="549" spans="3:4">
+      <c r="C549" s="1"/>
+      <c r="D549" s="1"/>
+    </row>
+    <row r="550" spans="3:4">
+      <c r="C550" s="1"/>
+      <c r="D550" s="1"/>
+    </row>
+    <row r="551" spans="3:4">
+      <c r="C551" s="1"/>
+      <c r="D551" s="1"/>
+    </row>
+    <row r="552" spans="3:4">
+      <c r="C552" s="1"/>
+      <c r="D552" s="1"/>
+    </row>
+    <row r="553" spans="3:4">
+      <c r="C553" s="1"/>
+      <c r="D553" s="1"/>
+    </row>
+    <row r="554" spans="3:4">
+      <c r="C554" s="1"/>
+      <c r="D554" s="1"/>
+    </row>
+    <row r="555" spans="3:4">
+      <c r="C555" s="1"/>
+      <c r="D555" s="1"/>
     </row>
     <row r="556" spans="3:4">
       <c r="C556" s="1"/>
@@ -44178,41 +44305,9 @@
       <c r="C2791" s="1"/>
       <c r="D2791" s="1"/>
     </row>
-    <row r="2792" spans="3:4">
-      <c r="C2792" s="1"/>
-      <c r="D2792" s="1"/>
-    </row>
-    <row r="2793" spans="3:4">
-      <c r="C2793" s="1"/>
-      <c r="D2793" s="1"/>
-    </row>
-    <row r="2794" spans="3:4">
-      <c r="C2794" s="1"/>
-      <c r="D2794" s="1"/>
-    </row>
-    <row r="2795" spans="3:4">
-      <c r="C2795" s="1"/>
-      <c r="D2795" s="1"/>
-    </row>
-    <row r="2796" spans="3:4">
-      <c r="C2796" s="1"/>
-      <c r="D2796" s="1"/>
-    </row>
-    <row r="2797" spans="3:4">
-      <c r="C2797" s="1"/>
-      <c r="D2797" s="1"/>
-    </row>
-    <row r="2798" spans="3:4">
-      <c r="C2798" s="1"/>
-      <c r="D2798" s="1"/>
-    </row>
-    <row r="2799" spans="3:4">
-      <c r="C2799" s="1"/>
-      <c r="D2799" s="1"/>
-    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B556:B2799 B7:B510">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B548:B2791 B7:B502">
       <formula1>OverridesDataTypeList</formula1>
     </dataValidation>
   </dataValidations>
@@ -44478,7 +44573,7 @@
     <row r="15" spans="1:5">
       <c r="A15" t="str">
         <f t="shared" si="0"/>
-        <v>NO</v>
+        <v>YES</v>
       </c>
       <c r="B15" s="67" t="str">
         <f t="shared" si="3"/>
@@ -44496,7 +44591,7 @@
     <row r="16" spans="1:5">
       <c r="A16" t="str">
         <f t="shared" si="0"/>
-        <v>NO</v>
+        <v>YES</v>
       </c>
       <c r="B16" s="67" t="str">
         <f t="shared" si="3"/>
@@ -44514,7 +44609,7 @@
     <row r="17" spans="1:4">
       <c r="A17" t="str">
         <f t="shared" si="0"/>
-        <v>NO</v>
+        <v>YES</v>
       </c>
       <c r="B17" s="67" t="str">
         <f t="shared" si="3"/>
@@ -44532,7 +44627,7 @@
     <row r="18" spans="1:4">
       <c r="A18" t="str">
         <f t="shared" si="0"/>
-        <v>NO</v>
+        <v>YES</v>
       </c>
       <c r="B18" s="67" t="str">
         <f t="shared" si="3"/>
@@ -44550,7 +44645,7 @@
     <row r="19" spans="1:4">
       <c r="A19" t="str">
         <f t="shared" si="0"/>
-        <v>NO</v>
+        <v>YES</v>
       </c>
       <c r="B19" s="67" t="str">
         <f t="shared" si="3"/>
@@ -44568,7 +44663,7 @@
     <row r="20" spans="1:4">
       <c r="A20" t="str">
         <f t="shared" si="0"/>
-        <v>NO</v>
+        <v>YES</v>
       </c>
       <c r="B20" s="67" t="str">
         <f t="shared" si="3"/>
@@ -44586,7 +44681,7 @@
     <row r="21" spans="1:4">
       <c r="A21" t="str">
         <f t="shared" si="0"/>
-        <v>NO</v>
+        <v>YES</v>
       </c>
       <c r="B21" s="67" t="str">
         <f t="shared" si="3"/>
@@ -44604,7 +44699,7 @@
     <row r="22" spans="1:4">
       <c r="A22" t="str">
         <f t="shared" si="0"/>
-        <v>NO</v>
+        <v>YES</v>
       </c>
       <c r="B22" s="67" t="str">
         <f t="shared" si="3"/>
@@ -44622,7 +44717,7 @@
     <row r="23" spans="1:4">
       <c r="A23" t="str">
         <f t="shared" si="0"/>
-        <v>NO</v>
+        <v>YES</v>
       </c>
       <c r="B23" s="67" t="str">
         <f t="shared" si="3"/>

</xml_diff>